<commit_message>
hl60 RNA-seq 72h used instead of 120h
</commit_message>
<xml_diff>
--- a/combined_analysis/intersectional-genes/Rho_down & Exp_down & Hyper_m6A.xlsx
+++ b/combined_analysis/intersectional-genes/Rho_down & Exp_down & Hyper_m6A.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
   <si>
     <t>chr</t>
   </si>
@@ -99,9 +99,6 @@
     <t>RGS19</t>
   </si>
   <si>
-    <t>MTF1</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
@@ -114,18 +111,12 @@
     <t>49</t>
   </si>
   <si>
-    <t>36,14</t>
-  </si>
-  <si>
     <t>0,2460</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>0,814</t>
-  </si>
-  <si>
     <t>ENSG00000083799.17</t>
   </si>
   <si>
@@ -147,9 +138,6 @@
     <t>ENSG00000171700.14</t>
   </si>
   <si>
-    <t>ENSG00000188786.10</t>
-  </si>
-  <si>
     <t>Exp.hl60.log2FC</t>
   </si>
   <si>
@@ -184,42 +172,6 @@
   </si>
   <si>
     <t>Exp.thp1.pval</t>
-  </si>
-  <si>
-    <t>Stbl.hl60.logFC</t>
-  </si>
-  <si>
-    <t>Stbl.hl60.pval</t>
-  </si>
-  <si>
-    <t>Stbl.kg1.logFC</t>
-  </si>
-  <si>
-    <t>Stbl.kg1.pval</t>
-  </si>
-  <si>
-    <t>Stbl.molm14.logFC</t>
-  </si>
-  <si>
-    <t>Stbl.molm14.pval</t>
-  </si>
-  <si>
-    <t>Stbl.ociaml2.logFC</t>
-  </si>
-  <si>
-    <t>Stbl.ociaml2.pval</t>
-  </si>
-  <si>
-    <t>Stbl.ociaml3.logFC</t>
-  </si>
-  <si>
-    <t>Stbl.ociaml3.pval</t>
-  </si>
-  <si>
-    <t>Stbl.thp1.logFC</t>
-  </si>
-  <si>
-    <t>Stbl.thp1.pval</t>
   </si>
   <si>
     <t>TE.Estimate_treatmentDRUG</t>
@@ -619,7 +571,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -689,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2">
         <v>50751859</v>
@@ -704,10 +656,10 @@
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M2">
         <v>4.64439089914138</v>
@@ -716,7 +668,7 @@
         <v>0.00280241217405675</v>
       </c>
       <c r="O2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -736,7 +688,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3">
         <v>130143817</v>
@@ -751,10 +703,10 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M3">
         <v>4.564348191458469</v>
@@ -763,7 +715,7 @@
         <v>2.36040070378252E-07</v>
       </c>
       <c r="O3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -783,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>10420064</v>
@@ -798,10 +750,10 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M4">
         <v>5.63121178182137</v>
@@ -810,7 +762,7 @@
         <v>0.000472983053087073</v>
       </c>
       <c r="O4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -830,7 +782,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5">
         <v>150577084</v>
@@ -845,10 +797,10 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M5">
         <v>1.70976450252654</v>
@@ -857,7 +809,7 @@
         <v>0.0008933596561736529</v>
       </c>
       <c r="O5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -877,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>150577332</v>
@@ -892,10 +844,10 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M6">
         <v>1.13284546031035</v>
@@ -904,7 +856,7 @@
         <v>0.00219156380531638</v>
       </c>
       <c r="O6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -924,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7">
         <v>150578994</v>
@@ -939,10 +891,10 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M7">
         <v>-0.6120544814950101</v>
@@ -951,7 +903,7 @@
         <v>0.0008583862741270429</v>
       </c>
       <c r="O7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -971,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8">
         <v>180610330</v>
@@ -986,10 +938,10 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M8">
         <v>5.49716822528384</v>
@@ -998,7 +950,7 @@
         <v>2.01589608117558E-07</v>
       </c>
       <c r="O8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1018,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9">
         <v>196353410</v>
@@ -1033,10 +985,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M9">
         <v>4.99721227842861</v>
@@ -1045,7 +997,7 @@
         <v>5.99989303866621E-05</v>
       </c>
       <c r="O9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1065,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>64073626</v>
@@ -1080,10 +1032,10 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M10">
         <v>5.00394630594547</v>
@@ -1092,101 +1044,7 @@
         <v>0.0014793526464042</v>
       </c>
       <c r="O10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>37822305</v>
-      </c>
-      <c r="C11">
-        <v>37822354</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11">
-        <v>37822305</v>
-      </c>
-      <c r="H11">
-        <v>37822354</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L11" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11">
-        <v>5.45532111534834</v>
-      </c>
-      <c r="N11">
-        <v>9.373188899486349E-07</v>
-      </c>
-      <c r="O11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>37857674</v>
-      </c>
-      <c r="C12">
-        <v>37858501</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12">
-        <v>37857674</v>
-      </c>
-      <c r="H12">
-        <v>37858501</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>2</v>
-      </c>
-      <c r="K12" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12">
-        <v>-1.74296930505857</v>
-      </c>
-      <c r="N12">
-        <v>0.000485927010331788</v>
-      </c>
-      <c r="O12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1196,275 +1054,203 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27">
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>-0.273</v>
+      </c>
+      <c r="C2">
+        <v>0.007</v>
+      </c>
+      <c r="D2">
+        <v>0.132</v>
+      </c>
+      <c r="E2">
+        <v>0.352</v>
+      </c>
+      <c r="F2">
+        <v>0.243</v>
+      </c>
+      <c r="G2">
+        <v>0.073</v>
+      </c>
+      <c r="H2">
+        <v>0.083</v>
+      </c>
+      <c r="I2">
+        <v>0.538</v>
+      </c>
+      <c r="J2">
+        <v>-0.163</v>
+      </c>
+      <c r="K2">
+        <v>0.289</v>
+      </c>
+      <c r="L2">
+        <v>0.124</v>
+      </c>
+      <c r="M2">
+        <v>0.353</v>
+      </c>
+      <c r="N2">
+        <v>-0.113</v>
+      </c>
+      <c r="O2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>-0.499</v>
+      </c>
+      <c r="C3">
+        <v>0.001</v>
+      </c>
+      <c r="D3">
+        <v>0.093</v>
+      </c>
+      <c r="E3">
+        <v>0.728</v>
+      </c>
+      <c r="F3">
+        <v>0.266</v>
+      </c>
+      <c r="G3">
+        <v>0.307</v>
+      </c>
+      <c r="H3">
+        <v>0.328</v>
+      </c>
+      <c r="I3">
+        <v>0.094</v>
+      </c>
+      <c r="J3">
+        <v>0.599</v>
+      </c>
+      <c r="K3">
+        <v>0.103</v>
+      </c>
+      <c r="L3">
+        <v>0.188</v>
+      </c>
+      <c r="M3">
+        <v>0.316</v>
+      </c>
+      <c r="N3">
+        <v>-0.132</v>
+      </c>
+      <c r="O3">
+        <v>0.927</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2">
-        <v>-1.566</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
+      <c r="B4">
+        <v>-1.291</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>-0.055</v>
       </c>
-      <c r="E2">
+      <c r="E4">
         <v>0.733</v>
       </c>
-      <c r="F2">
+      <c r="F4">
         <v>0.45</v>
       </c>
-      <c r="G2">
+      <c r="G4">
         <v>0.081</v>
       </c>
-      <c r="H2">
+      <c r="H4">
         <v>-0.046</v>
       </c>
-      <c r="I2">
+      <c r="I4">
         <v>0.828</v>
       </c>
-      <c r="J2">
+      <c r="J4">
         <v>0.382</v>
       </c>
-      <c r="K2">
+      <c r="K4">
         <v>0.098</v>
       </c>
-      <c r="L2">
+      <c r="L4">
         <v>-0.286</v>
       </c>
-      <c r="M2">
+      <c r="M4">
         <v>0.257</v>
       </c>
-      <c r="Z2">
+      <c r="N4">
         <v>-0.326</v>
       </c>
-      <c r="AA2">
+      <c r="O4">
         <v>0.766</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3">
-        <v>-0.483</v>
-      </c>
-      <c r="C3">
-        <v>0.007</v>
-      </c>
-      <c r="D3">
-        <v>0.132</v>
-      </c>
-      <c r="E3">
-        <v>0.352</v>
-      </c>
-      <c r="F3">
-        <v>0.243</v>
-      </c>
-      <c r="G3">
-        <v>0.073</v>
-      </c>
-      <c r="H3">
-        <v>0.083</v>
-      </c>
-      <c r="I3">
-        <v>0.538</v>
-      </c>
-      <c r="J3">
-        <v>-0.163</v>
-      </c>
-      <c r="K3">
-        <v>0.289</v>
-      </c>
-      <c r="L3">
-        <v>0.124</v>
-      </c>
-      <c r="M3">
-        <v>0.353</v>
-      </c>
-      <c r="Z3">
-        <v>-0.113</v>
-      </c>
-      <c r="AA3">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <v>-0.235</v>
-      </c>
-      <c r="C4">
-        <v>0.001</v>
-      </c>
-      <c r="D4">
-        <v>0.093</v>
-      </c>
-      <c r="E4">
-        <v>0.728</v>
-      </c>
-      <c r="F4">
-        <v>0.266</v>
-      </c>
-      <c r="G4">
-        <v>0.307</v>
-      </c>
-      <c r="H4">
-        <v>0.328</v>
-      </c>
-      <c r="I4">
-        <v>0.094</v>
-      </c>
-      <c r="J4">
-        <v>0.599</v>
-      </c>
-      <c r="K4">
-        <v>0.103</v>
-      </c>
-      <c r="L4">
-        <v>0.188</v>
-      </c>
-      <c r="M4">
-        <v>0.316</v>
-      </c>
-      <c r="N4">
-        <v>0.289</v>
-      </c>
-      <c r="O4">
-        <v>0.064</v>
-      </c>
-      <c r="P4">
-        <v>-0.045</v>
-      </c>
-      <c r="Q4">
-        <v>0.702</v>
-      </c>
-      <c r="R4">
-        <v>0.108</v>
-      </c>
-      <c r="S4">
-        <v>0.469</v>
-      </c>
-      <c r="T4">
-        <v>0.171</v>
-      </c>
-      <c r="U4">
-        <v>0.12</v>
-      </c>
-      <c r="V4">
-        <v>-0.203</v>
-      </c>
-      <c r="W4">
-        <v>0.169</v>
-      </c>
-      <c r="X4">
-        <v>0.133</v>
-      </c>
-      <c r="Y4">
-        <v>0.218</v>
-      </c>
-      <c r="Z4">
-        <v>-0.132</v>
-      </c>
-      <c r="AA4">
-        <v>0.927</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
-        <v>-0.785</v>
+        <v>-1.096</v>
       </c>
       <c r="C5">
         <v>0.004</v>
@@ -1500,101 +1286,65 @@
         <v>0.311</v>
       </c>
       <c r="N5">
-        <v>0.429</v>
+        <v>0.1</v>
       </c>
       <c r="O5">
-        <v>0.005</v>
-      </c>
-      <c r="P5">
-        <v>-0.002</v>
-      </c>
-      <c r="Q5">
+        <v>0.667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>-0.435</v>
+      </c>
+      <c r="C6">
+        <v>0.001</v>
+      </c>
+      <c r="D6">
+        <v>-0.073</v>
+      </c>
+      <c r="E6">
+        <v>0.653</v>
+      </c>
+      <c r="F6">
+        <v>0.506</v>
+      </c>
+      <c r="G6">
+        <v>0.023</v>
+      </c>
+      <c r="H6">
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="I6">
+        <v>0.58</v>
+      </c>
+      <c r="J6">
+        <v>-0.004</v>
+      </c>
+      <c r="K6">
         <v>0.987</v>
       </c>
-      <c r="R5">
-        <v>0.111</v>
-      </c>
-      <c r="S5">
-        <v>0.352</v>
-      </c>
-      <c r="T5">
-        <v>0.168</v>
-      </c>
-      <c r="U5">
-        <v>0.126</v>
-      </c>
-      <c r="V5">
-        <v>0.309</v>
-      </c>
-      <c r="W5">
-        <v>0.061</v>
-      </c>
-      <c r="X5">
-        <v>-0.074</v>
-      </c>
-      <c r="Y5">
-        <v>0.45</v>
-      </c>
-      <c r="Z5">
-        <v>0.1</v>
-      </c>
-      <c r="AA5">
-        <v>0.667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6">
-        <v>-0.157</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0.016</v>
-      </c>
-      <c r="E6">
-        <v>0.9370000000000001</v>
-      </c>
-      <c r="F6">
-        <v>-0.447</v>
-      </c>
-      <c r="G6">
-        <v>0.214</v>
-      </c>
-      <c r="H6">
-        <v>0.305</v>
-      </c>
-      <c r="I6">
-        <v>0.204</v>
-      </c>
-      <c r="J6">
-        <v>0.002</v>
-      </c>
-      <c r="K6">
-        <v>0.994</v>
-      </c>
       <c r="L6">
-        <v>0.283</v>
+        <v>-0.359</v>
       </c>
       <c r="M6">
-        <v>0.204</v>
-      </c>
-      <c r="Z6">
-        <v>0.124</v>
-      </c>
-      <c r="AA6">
-        <v>0.9399999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27">
+        <v>0.034</v>
+      </c>
+      <c r="N6">
+        <v>-0.111</v>
+      </c>
+      <c r="O6">
+        <v>0.922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B7">
-        <v>-1.797</v>
+        <v>-1.76</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1630,49 +1380,13 @@
         <v>0.035</v>
       </c>
       <c r="N7">
-        <v>0.279</v>
+        <v>-0.089</v>
       </c>
       <c r="O7">
-        <v>0.114</v>
-      </c>
-      <c r="P7">
-        <v>0.005</v>
-      </c>
-      <c r="Q7">
-        <v>0.961</v>
-      </c>
-      <c r="R7">
-        <v>0.008999999999999999</v>
-      </c>
-      <c r="S7">
-        <v>0.949</v>
-      </c>
-      <c r="T7">
-        <v>-0.101</v>
-      </c>
-      <c r="U7">
-        <v>0.39</v>
-      </c>
-      <c r="V7">
-        <v>-0.337</v>
-      </c>
-      <c r="W7">
-        <v>0.067</v>
-      </c>
-      <c r="X7">
-        <v>-0.183</v>
-      </c>
-      <c r="Y7">
-        <v>0.112</v>
-      </c>
-      <c r="Z7">
-        <v>-0.089</v>
-      </c>
-      <c r="AA7">
         <v>0.8110000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1712,94 +1426,11 @@
       <c r="M8">
         <v>0.314</v>
       </c>
-      <c r="Z8">
+      <c r="N8">
         <v>0.108</v>
       </c>
-      <c r="AA8">
+      <c r="O8">
         <v>0.928</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
-        <v>-0.284</v>
-      </c>
-      <c r="C9">
-        <v>0.001</v>
-      </c>
-      <c r="D9">
-        <v>-0.073</v>
-      </c>
-      <c r="E9">
-        <v>0.653</v>
-      </c>
-      <c r="F9">
-        <v>0.506</v>
-      </c>
-      <c r="G9">
-        <v>0.023</v>
-      </c>
-      <c r="H9">
-        <v>0.08500000000000001</v>
-      </c>
-      <c r="I9">
-        <v>0.58</v>
-      </c>
-      <c r="J9">
-        <v>-0.004</v>
-      </c>
-      <c r="K9">
-        <v>0.987</v>
-      </c>
-      <c r="L9">
-        <v>-0.359</v>
-      </c>
-      <c r="M9">
-        <v>0.034</v>
-      </c>
-      <c r="N9">
-        <v>0.1</v>
-      </c>
-      <c r="O9">
-        <v>0.424</v>
-      </c>
-      <c r="P9">
-        <v>-0.101</v>
-      </c>
-      <c r="Q9">
-        <v>0.42</v>
-      </c>
-      <c r="R9">
-        <v>-0.104</v>
-      </c>
-      <c r="S9">
-        <v>0.348</v>
-      </c>
-      <c r="T9">
-        <v>-0.064</v>
-      </c>
-      <c r="U9">
-        <v>0.574</v>
-      </c>
-      <c r="V9">
-        <v>-0.177</v>
-      </c>
-      <c r="W9">
-        <v>0.23</v>
-      </c>
-      <c r="X9">
-        <v>-0.354</v>
-      </c>
-      <c r="Y9">
-        <v>0.026</v>
-      </c>
-      <c r="Z9">
-        <v>-0.111</v>
-      </c>
-      <c r="AA9">
-        <v>0.922</v>
       </c>
     </row>
   </sheetData>
@@ -1809,7 +1440,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1820,163 +1451,163 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>-0.246</v>
       </c>
       <c r="C2">
+        <v>0.027</v>
+      </c>
+      <c r="D2">
+        <v>-0.266</v>
+      </c>
+      <c r="E2">
+        <v>0.023</v>
+      </c>
+      <c r="F2">
+        <v>-0.228</v>
+      </c>
+      <c r="G2">
+        <v>0.14</v>
+      </c>
+      <c r="H2">
+        <v>-0.152</v>
+      </c>
+      <c r="I2">
         <v>0.001</v>
       </c>
-      <c r="D2">
-        <v>-0.232</v>
-      </c>
-      <c r="E2">
-        <v>0.068</v>
-      </c>
-      <c r="F2">
-        <v>-0.173</v>
-      </c>
-      <c r="G2">
-        <v>0.076</v>
-      </c>
-      <c r="H2">
-        <v>0.023</v>
-      </c>
-      <c r="I2">
-        <v>0.424</v>
-      </c>
       <c r="J2">
-        <v>0.099</v>
+        <v>-0.183</v>
       </c>
       <c r="K2">
-        <v>0.093</v>
+        <v>0.004</v>
       </c>
       <c r="L2">
-        <v>0.099</v>
+        <v>-0.183</v>
       </c>
       <c r="M2">
-        <v>0.093</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>-0.246</v>
+        <v>-0.182</v>
       </c>
       <c r="C3">
-        <v>0.027</v>
+        <v>0.004</v>
       </c>
       <c r="D3">
-        <v>-0.266</v>
+        <v>-0.167</v>
       </c>
       <c r="E3">
-        <v>0.023</v>
+        <v>0.078</v>
       </c>
       <c r="F3">
-        <v>-0.228</v>
+        <v>-0.123</v>
       </c>
       <c r="G3">
-        <v>0.14</v>
+        <v>0.235</v>
       </c>
       <c r="H3">
-        <v>-0.152</v>
+        <v>-0.001</v>
       </c>
       <c r="I3">
-        <v>0.001</v>
+        <v>0.8</v>
       </c>
       <c r="J3">
-        <v>-0.183</v>
+        <v>-0.048</v>
       </c>
       <c r="K3">
-        <v>0.004</v>
+        <v>0.131</v>
       </c>
       <c r="L3">
-        <v>-0.183</v>
+        <v>-0.048</v>
       </c>
       <c r="M3">
-        <v>0.004</v>
+        <v>0.131</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>-0.182</v>
+        <v>-0.246</v>
       </c>
       <c r="C4">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="D4">
-        <v>-0.167</v>
+        <v>-0.232</v>
       </c>
       <c r="E4">
-        <v>0.078</v>
+        <v>0.068</v>
       </c>
       <c r="F4">
-        <v>-0.123</v>
+        <v>-0.173</v>
       </c>
       <c r="G4">
-        <v>0.235</v>
+        <v>0.076</v>
       </c>
       <c r="H4">
-        <v>-0.001</v>
+        <v>0.023</v>
       </c>
       <c r="I4">
-        <v>0.8</v>
+        <v>0.424</v>
       </c>
       <c r="J4">
-        <v>-0.048</v>
+        <v>0.099</v>
       </c>
       <c r="K4">
-        <v>0.131</v>
+        <v>0.093</v>
       </c>
       <c r="L4">
-        <v>-0.048</v>
+        <v>0.099</v>
       </c>
       <c r="M4">
-        <v>0.131</v>
+        <v>0.093</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2022,43 +1653,43 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6">
-        <v>-0.297</v>
+        <v>-0.106</v>
       </c>
       <c r="C6">
-        <v>0.002</v>
+        <v>0.357</v>
       </c>
       <c r="D6">
-        <v>-0.262</v>
+        <v>-0.201</v>
       </c>
       <c r="E6">
-        <v>0.012</v>
+        <v>0.005</v>
       </c>
       <c r="F6">
-        <v>-0.254</v>
+        <v>-0.267</v>
       </c>
       <c r="G6">
-        <v>0.064</v>
+        <v>0.013</v>
       </c>
       <c r="H6">
-        <v>-0.147</v>
+        <v>0.042</v>
       </c>
       <c r="I6">
-        <v>0.138</v>
+        <v>0.11</v>
       </c>
       <c r="J6">
-        <v>-0.134</v>
+        <v>0.038</v>
       </c>
       <c r="K6">
-        <v>0.823</v>
+        <v>0.62</v>
       </c>
       <c r="L6">
-        <v>-0.134</v>
+        <v>0.038</v>
       </c>
       <c r="M6">
-        <v>0.823</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2141,47 +1772,6 @@
       </c>
       <c r="M8">
         <v>0.052</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
-        <v>-0.106</v>
-      </c>
-      <c r="C9">
-        <v>0.357</v>
-      </c>
-      <c r="D9">
-        <v>-0.201</v>
-      </c>
-      <c r="E9">
-        <v>0.005</v>
-      </c>
-      <c r="F9">
-        <v>-0.267</v>
-      </c>
-      <c r="G9">
-        <v>0.013</v>
-      </c>
-      <c r="H9">
-        <v>0.042</v>
-      </c>
-      <c r="I9">
-        <v>0.11</v>
-      </c>
-      <c r="J9">
-        <v>0.038</v>
-      </c>
-      <c r="K9">
-        <v>0.62</v>
-      </c>
-      <c r="L9">
-        <v>0.038</v>
-      </c>
-      <c r="M9">
-        <v>0.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>